<commit_message>
Fix full size and AF output for weather clusters
</commit_message>
<xml_diff>
--- a/Clustering/Output_Clusters_Asigned_To_Countries/kmeans_10_af_df_solar.xlsx
+++ b/Clustering/Output_Clusters_Asigned_To_Countries/kmeans_10_af_df_solar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,6 +458,9 @@
       <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -475,19 +478,22 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01263243683781581</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.003528581510232887</v>
       </c>
       <c r="G2" t="n">
-        <v>0.006302521008403361</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.01909241837299393</v>
       </c>
     </row>
     <row r="3">
@@ -497,28 +503,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.1443066516347239</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2272727272727271</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02893235533822326</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.001411432604093155</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002100840336134454</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1280000000000001</v>
+        <v>0.2382528127068175</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.02296624239070285</v>
       </c>
     </row>
     <row r="4">
@@ -531,25 +540,28 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.1057692307692306</v>
       </c>
       <c r="D4" t="n">
-        <v>0.06666666666666667</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05916305916305913</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.07317073170731707</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1099099099099098</v>
+        <v>0.06159895150720845</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -559,28 +571,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.0541149943630213</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1407624633431084</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.08109209453952747</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.04446012702893437</v>
       </c>
       <c r="G5" t="n">
-        <v>0.06932773109243705</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0384</v>
+        <v>0.02117802779616148</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.05368013281682354</v>
       </c>
     </row>
     <row r="6">
@@ -599,19 +614,22 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02648736756316215</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.003528581510232887</v>
       </c>
       <c r="G6" t="n">
-        <v>0.005252100840336134</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.02877697841726622</v>
       </c>
     </row>
     <row r="7">
@@ -621,19 +639,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.008676789587852495</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.01736972704714641</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1139971139971139</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -642,6 +660,9 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
+        <v>0.1441677588466578</v>
+      </c>
+      <c r="J7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -652,28 +673,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.08399098083427288</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2126099706744866</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.08924205378973125</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.01199717713479181</v>
       </c>
       <c r="G8" t="n">
-        <v>0.02100840336134454</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4175999999999984</v>
+        <v>0.2183984116479159</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.05838406198118436</v>
       </c>
     </row>
     <row r="9">
@@ -683,27 +707,30 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1876355748373104</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.2142266335814727</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.02328863796753705</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01680672268907563</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
+        <v>0.01048492791612058</v>
+      </c>
+      <c r="J9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -717,25 +744,28 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.1038461538461537</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1125541125541124</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.1219512195121951</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1099099099099098</v>
+        <v>0.1153342070773263</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -745,27 +775,30 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.001084598698481562</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.0008271298593879239</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.01764290755116443</v>
       </c>
       <c r="G11" t="n">
-        <v>0.02626050420168067</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -776,27 +809,30 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.03687635574837313</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.02646815550041358</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02020202020202021</v>
+        <v>0.0155257586450247</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01995798319327731</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
+        <v>0.01703800786369594</v>
+      </c>
+      <c r="J12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -816,19 +852,22 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01874490627546862</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.009174311926605505</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01470588235294117</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.01300498063087992</v>
       </c>
     </row>
     <row r="14">
@@ -838,28 +877,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>0.0259301014656144</v>
       </c>
       <c r="C14" t="n">
-        <v>0.06304985337243399</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01792991035044824</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>0.0007057163020465773</v>
       </c>
       <c r="G14" t="n">
-        <v>0.001050420168067227</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.0113447703375761</v>
       </c>
     </row>
     <row r="15">
@@ -892,6 +934,9 @@
       <c r="I15" t="n">
         <v>0</v>
       </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -900,28 +945,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2440347071583521</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.01153846153846154</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>0.1819685690653434</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03993480032599835</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1370851370851369</v>
+        <v>0.2173606210303458</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3203781512605034</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01981981981981982</v>
+        <v>0.1284403669724769</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.02822357498616495</v>
       </c>
     </row>
     <row r="17">
@@ -940,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.03871230643846778</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -953,6 +1001,9 @@
       </c>
       <c r="I17" t="n">
         <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.02767017155506368</v>
       </c>
     </row>
     <row r="18">
@@ -962,19 +1013,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01193058568329718</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>0.009925558312655087</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0101010101010101</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -983,6 +1034,9 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
+        <v>0.007863695937090432</v>
+      </c>
+      <c r="J18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1002,19 +1056,22 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01385493072534638</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.02399435426958363</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03886554621848742</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.01023796347537356</v>
       </c>
     </row>
     <row r="20">
@@ -1024,28 +1081,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.001691093573844419</v>
       </c>
       <c r="C20" t="n">
-        <v>0.001466275659824047</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1837815810920952</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.006351446718419196</v>
       </c>
       <c r="G20" t="n">
-        <v>0.009453781512605041</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.1242390702822359</v>
       </c>
     </row>
     <row r="21">
@@ -1055,28 +1115,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.002169197396963124</v>
+        <v>0.02085682074408116</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01173020527859238</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>0.001654259718775848</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1727791361043201</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.05363443895553988</v>
       </c>
       <c r="G21" t="n">
-        <v>0.08193277310924373</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.1098505810736028</v>
       </c>
     </row>
     <row r="22">
@@ -1109,6 +1172,9 @@
       <c r="I22" t="n">
         <v>0</v>
       </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1117,28 +1183,31 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>0.1104847801578357</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2976539589442813</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1564792176039125</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.02117148906139732</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0346638655462185</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0.3871999999999985</v>
+        <v>0.170747849106552</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.1045932484781407</v>
       </c>
     </row>
     <row r="24">
@@ -1154,13 +1223,13 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.0008271298593879239</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.04906204906204904</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1169,6 +1238,9 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
+        <v>0.0432503276539974</v>
+      </c>
+      <c r="J24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1179,27 +1251,30 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.06182212581344908</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.04549214226633585</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>0.04940014114326041</v>
       </c>
       <c r="G25" t="n">
-        <v>0.07142857142857149</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1210,13 +1285,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.001084598698481562</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>0.0008271298593879239</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1231,6 +1306,9 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1241,27 +1319,30 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.0260303687635575</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>0.01902398676592226</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.02308802308802309</v>
+        <v>0.01129146083274524</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01470588235294117</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
       <c r="I27" t="n">
+        <v>0.01965923984272608</v>
+      </c>
+      <c r="J27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1281,19 +1362,22 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>0.03789731051344741</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>0.01270289343683839</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02100840336134454</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.02628666297731049</v>
       </c>
     </row>
     <row r="29">
@@ -1312,19 +1396,22 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.003667481662591687</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>0.03881439661256175</v>
       </c>
       <c r="G29" t="n">
-        <v>0.05777310924369756</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.002490315439955728</v>
       </c>
     </row>
     <row r="30">
@@ -1334,27 +1421,30 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.02928416485900219</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>0.02233250620347396</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.001443001443001443</v>
+        <v>0.05645730416372619</v>
       </c>
       <c r="G30" t="n">
-        <v>0.08403361344537817</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
+        <v>0.001310615989515072</v>
+      </c>
+      <c r="J30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1365,19 +1455,19 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.09544468546637734</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>0.07526881720430104</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.03607503607503608</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1386,6 +1476,9 @@
         <v>0</v>
       </c>
       <c r="I31" t="n">
+        <v>0.02883355176933158</v>
+      </c>
+      <c r="J31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1396,28 +1489,31 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.07917570498915399</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>0.6365384615384595</v>
       </c>
       <c r="D32" t="n">
-        <v>0.8333333333333324</v>
+        <v>0.06534325889164602</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.1616161616161614</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>0.8048780487804883</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>0.6054054054054023</v>
+        <v>0.1572739187418084</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1427,28 +1523,31 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.158351409978308</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>0.142307692307692</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>0.1248966087675761</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2121212121212118</v>
+        <v>0.004234297812279464</v>
       </c>
       <c r="G33" t="n">
-        <v>0.005252100840336134</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>0.154954954954955</v>
+        <v>0.2005242463958057</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1467,19 +1566,22 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01711491442542787</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>0.0007057163020465773</v>
       </c>
       <c r="G34" t="n">
-        <v>0.001050420168067227</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.01162147205312674</v>
       </c>
     </row>
     <row r="35">
@@ -1489,182 +1591,30 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.05639913232104127</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>0.04383788254756</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.01154401154401154</v>
+        <v>0.002117148906139732</v>
       </c>
       <c r="G35" t="n">
-        <v>0.002100840336134454</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>Joint regime area Spain / France</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>Joint regime area United Kingdom / Denmark (Faeroe Islands)</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Joint regime area Italy / France</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>Joint regime area Sweden / Norway</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Joint regime area Croatia / Slovenia</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" t="n">
+        <v>0.007863695937090432</v>
+      </c>
+      <c r="J35" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>